<commit_message>
Added charts on main page
</commit_message>
<xml_diff>
--- a/Assets_Revenues_Benefits/assets_data.xlsx
+++ b/Assets_Revenues_Benefits/assets_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Konstantinos\Desktop\CS projects\Hackathons\Bankrupt_Smart_Code\Assets_Revenues_Benefits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469086C9-8E60-46E3-8F6C-AA067E7F6C56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3FF416-02D7-440A-88B4-D2E35D8A2A88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{596D3C95-C05C-4457-81C9-B35EB9C2DA46}"/>
   </bookViews>
@@ -439,7 +439,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,7 +541,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>1250</v>
+        <v>800</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -592,7 +592,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1250</v>
+        <v>3368</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -643,7 +643,7 @@
         <v>7</v>
       </c>
       <c r="B12">
-        <v>1250</v>
+        <v>455</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -694,7 +694,7 @@
         <v>7</v>
       </c>
       <c r="B15">
-        <v>1250</v>
+        <v>1356</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -745,7 +745,7 @@
         <v>7</v>
       </c>
       <c r="B18">
-        <v>1250</v>
+        <v>685</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -796,7 +796,7 @@
         <v>7</v>
       </c>
       <c r="B21">
-        <v>1250</v>
+        <v>1125</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -847,7 +847,7 @@
         <v>7</v>
       </c>
       <c r="B24">
-        <v>1250</v>
+        <v>3358</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -898,7 +898,7 @@
         <v>7</v>
       </c>
       <c r="B27">
-        <v>1250</v>
+        <v>10</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -949,7 +949,7 @@
         <v>7</v>
       </c>
       <c r="B30">
-        <v>1250</v>
+        <v>258</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1000,7 +1000,7 @@
         <v>7</v>
       </c>
       <c r="B33">
-        <v>1250</v>
+        <v>3225</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1051,7 +1051,7 @@
         <v>7</v>
       </c>
       <c r="B36">
-        <v>1250</v>
+        <v>1890</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1090,7 +1090,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1530,7 +1530,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1602,8 +1602,7 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>280</v>
+        <v>250</v>
       </c>
       <c r="C6" s="1">
         <v>43952</v>
@@ -1615,7 +1614,7 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>270</v>
       </c>
       <c r="C7" s="1">
         <v>44013</v>
@@ -1626,8 +1625,7 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>320</v>
+        <v>200</v>
       </c>
       <c r="C8" s="1">
         <v>44075</v>
@@ -1639,7 +1637,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>340</v>
+        <v>220</v>
       </c>
       <c r="C9" s="1">
         <v>44105</v>
@@ -1651,7 +1649,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>360</v>
+        <v>240</v>
       </c>
       <c r="C10" s="1">
         <v>44136</v>
@@ -1663,7 +1661,7 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>380</v>
+        <v>260</v>
       </c>
       <c r="C11" s="1">
         <v>44166</v>

</xml_diff>